<commit_message>
Aanmaken project, navigatie en schermen
</commit_message>
<xml_diff>
--- a/Logboek_EilishVanDerSnickt.xlsx
+++ b/Logboek_EilishVanDerSnickt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\programs (D-schijf)\Github\MI4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DFD74AE-D991-40AA-9B49-8725985B33EB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53126CBB-59F9-471F-8282-A418BBD6C29B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5EE9FC85-C76D-4205-AD20-DF6E8E905733}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>MI4 - Logboek Eilish Van Der Snickt</t>
   </si>
@@ -70,6 +70,36 @@
   </si>
   <si>
     <t>https://developers.google.com/maps/documentation/android-sdk/location#the_my_location_layer</t>
+  </si>
+  <si>
+    <t>5 uur 30 minuten</t>
+  </si>
+  <si>
+    <t>week 2</t>
+  </si>
+  <si>
+    <t>Ervoor zorgen dat er maximaal 2 markers toegevoegt kunnen worden, de markers een andere opmaak geven</t>
+  </si>
+  <si>
+    <t>40 minuten</t>
+  </si>
+  <si>
+    <t>10 minuten</t>
+  </si>
+  <si>
+    <t>Teken een lijn tussen 2 markers</t>
+  </si>
+  <si>
+    <t>https://developers.google.com/maps/documentation/android-sdk/polygon-tutorial</t>
+  </si>
+  <si>
+    <t>https://app-privacy-policy-generator.firebaseapp.com/</t>
+  </si>
+  <si>
+    <t>https://firebase.google.com/docs/android/setup</t>
+  </si>
+  <si>
+    <t>Aanmaken project, navigatie toevoegen, schermen toevoegen, verder werken proefproject, polylines blijven updaten wanneer er een marker bij komt, de polyline updaten elke keer dat je locatie verandert</t>
   </si>
 </sst>
 </file>
@@ -452,10 +482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{119EAF89-ED89-44FA-A8CC-5183F94E79BB}">
-  <dimension ref="A1:Q8"/>
+  <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -473,7 +503,9 @@
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3"/>
+      <c r="B2" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
@@ -507,23 +539,69 @@
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="3"/>
       <c r="Q5" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>43514</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
       <c r="Q6" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>43516</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
       <c r="Q7" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>43518</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
       <c r="Q8" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q11" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
layout 1ste belangrijk scherm
</commit_message>
<xml_diff>
--- a/Logboek_EilishVanDerSnickt.xlsx
+++ b/Logboek_EilishVanDerSnickt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\programs (D-schijf)\Github\MI4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D1E018B-C975-4FBC-B75F-3A54BD267691}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7D6643F-4390-4457-A7BC-4CF2384562FB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5EE9FC85-C76D-4205-AD20-DF6E8E905733}"/>
   </bookViews>
@@ -117,10 +117,10 @@
     <t>https://developer.android.com/topic/libraries/architecture/navigation/navigation-implementing</t>
   </si>
   <si>
-    <t>1 uur 5 minuten</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aanmaken toast message op proefproject, navigatie tussen schermen op project en uittekenen details van de 3 belangrijkste schermen </t>
+    <t>1 uur 35 minuten</t>
+  </si>
+  <si>
+    <t>Aanmaken toast message op proefproject, navigatie tussen schermen op project en uittekenen details van de 3 belangrijkste schermen, aanmaken layout 1ste belangrijk scherm</t>
   </si>
 </sst>
 </file>
@@ -506,7 +506,7 @@
   <dimension ref="A1:Q12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Firebase Inloggen en wachtwoord vergeten, viewpager, cardview en recyclerview
</commit_message>
<xml_diff>
--- a/Logboek_EilishVanDerSnickt.xlsx
+++ b/Logboek_EilishVanDerSnickt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\programs (D-schijf)\Github\MI4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8E05AAE-64C8-4358-B27D-36C58B1CFB9C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1399961-CBA0-44D9-8445-5650143F2A6A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5EE9FC85-C76D-4205-AD20-DF6E8E905733}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
   <si>
     <t>MI4 - Logboek Eilish Van Der Snickt</t>
   </si>
@@ -133,6 +133,18 @@
   </si>
   <si>
     <t>Testen proefproject locatie, navigatie in klassen op project, firebase registratie aanmaken en testen</t>
+  </si>
+  <si>
+    <t>https://console.firebase.google.com/</t>
+  </si>
+  <si>
+    <t>https://www.androidhive.info/2015/09/android-material-design-working-with-tabs/</t>
+  </si>
+  <si>
+    <t>https://www.androidhive.info/2016/05/android-working-with-card-view-and-recycler-view/</t>
+  </si>
+  <si>
+    <t>Firebase inloggen en wachtwoord vergeten toepassen, viewpager aanmaken, cardview in recyclerview zetten, verder uitwerken schermen, cardview toevoegen</t>
   </si>
 </sst>
 </file>
@@ -515,10 +527,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{119EAF89-ED89-44FA-A8CC-5183F94E79BB}">
-  <dimension ref="A1:Q14"/>
+  <dimension ref="A1:Q17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P20" sqref="P20"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -675,6 +687,15 @@
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>43525</v>
+      </c>
+      <c r="B13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" t="s">
+        <v>37</v>
+      </c>
       <c r="Q13" t="s">
         <v>30</v>
       </c>
@@ -682,6 +703,21 @@
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="Q14" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q17" s="5" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -689,8 +725,9 @@
     <hyperlink ref="Q3" r:id="rId1" xr:uid="{6AAF29A2-E215-4421-B355-D6304BEF638E}"/>
     <hyperlink ref="Q5" r:id="rId2" xr:uid="{AE1F0DE4-AC8E-4ED9-965B-1293157AA6E7}"/>
     <hyperlink ref="Q4" r:id="rId3" xr:uid="{5AF087A5-6825-43E4-AF9C-97B4F0608956}"/>
+    <hyperlink ref="Q17" r:id="rId4" xr:uid="{6F8EE77C-DF59-467A-9123-382FE281C10A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Hoofdschermen uitwerken en navigatie ertussen
</commit_message>
<xml_diff>
--- a/Logboek_EilishVanDerSnickt.xlsx
+++ b/Logboek_EilishVanDerSnickt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\programs (D-schijf)\Github\MI4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{630B3CFD-2BF7-4155-9F44-6D17ADC21EB7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{058D4F50-8BEF-4CDD-83DA-219B677388A0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5EE9FC85-C76D-4205-AD20-DF6E8E905733}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="44">
   <si>
     <t>MI4 - Logboek Eilish Van Der Snickt</t>
   </si>
@@ -151,6 +151,18 @@
   </si>
   <si>
     <t>onLocationChangedListener testen in proefproject, viewpager werking oplossen in project, werking in klasses optimaliseren in project</t>
+  </si>
+  <si>
+    <t>Hoofdscherm project verder uitwerken, activiteit scherm aanmaken en opmaken, instellingen scherm aanmaken, navigatie tussen deze schermen</t>
+  </si>
+  <si>
+    <t>Week 4</t>
+  </si>
+  <si>
+    <t>10 uur 30 minuten</t>
+  </si>
+  <si>
+    <t>2 uur 15 minuten</t>
   </si>
 </sst>
 </file>
@@ -536,7 +548,7 @@
   <dimension ref="A1:Q17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -660,6 +672,9 @@
       <c r="A10" s="4" t="s">
         <v>26</v>
       </c>
+      <c r="B10" s="4" t="s">
+        <v>42</v>
+      </c>
       <c r="Q10" t="s">
         <v>20</v>
       </c>
@@ -721,11 +736,23 @@
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>41</v>
+      </c>
       <c r="Q15" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>43530</v>
+      </c>
+      <c r="B16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" t="s">
+        <v>40</v>
+      </c>
       <c r="Q16" t="s">
         <v>35</v>
       </c>

</xml_diff>

<commit_message>
Instellingenscherm en functionaliteiten toevoegen
</commit_message>
<xml_diff>
--- a/Logboek_EilishVanDerSnickt.xlsx
+++ b/Logboek_EilishVanDerSnickt.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\programs (D-schijf)\Github\MI4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{058D4F50-8BEF-4CDD-83DA-219B677388A0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6112EF0-93DF-40DA-BBC5-95525CA98366}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5EE9FC85-C76D-4205-AD20-DF6E8E905733}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
   <si>
     <t>MI4 - Logboek Eilish Van Der Snickt</t>
   </si>
@@ -163,6 +163,15 @@
   </si>
   <si>
     <t>2 uur 15 minuten</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=eX-TdY6bLdg</t>
+  </si>
+  <si>
+    <t>Week 5</t>
+  </si>
+  <si>
+    <t>Instellingen scherm verder uitwerken, navigatie aanpassen, popupscherm maken, gebruikers verwijderen en beginnende code voor wachtwoord wijziging</t>
   </si>
 </sst>
 </file>
@@ -545,10 +554,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{119EAF89-ED89-44FA-A8CC-5183F94E79BB}">
-  <dimension ref="A1:Q17"/>
+  <dimension ref="A1:Q18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -739,6 +748,9 @@
       <c r="A15" s="4" t="s">
         <v>41</v>
       </c>
+      <c r="B15" s="4" t="s">
+        <v>43</v>
+      </c>
       <c r="Q15" t="s">
         <v>34</v>
       </c>
@@ -757,9 +769,27 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="17:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" s="4"/>
       <c r="Q17" s="5" t="s">
         <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>43540</v>
+      </c>
+      <c r="B18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Aanmaken acitviteit op basis van locatie en navigatie
</commit_message>
<xml_diff>
--- a/Logboek_EilishVanDerSnickt.xlsx
+++ b/Logboek_EilishVanDerSnickt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\programs (D-schijf)\Github\MI4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{672AC1A1-524D-4548-9C57-4C663E768311}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A3D5ABC-2365-45F0-84FA-00C7B517C9D1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5EE9FC85-C76D-4205-AD20-DF6E8E905733}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="52">
   <si>
     <t>MI4 - Logboek Eilish Van Der Snickt</t>
   </si>
@@ -183,7 +183,10 @@
     <t>http://www.zoftino.com/android-mapview-tutorial</t>
   </si>
   <si>
-    <t>Instellingen wachtwoord wizigen, email aanmaken en uitloggen aanmaken, google maps view aanmaken, navigatie naar nieuw scherm</t>
+    <t>4 uur 30 minuten</t>
+  </si>
+  <si>
+    <t>Instellingen wachtwoord wizigen, email aanmaken en uitloggen aanmaken, google maps view aanmaken, navigatie naar nieuw scherm, nieuw scherm opmaken en navigatie regelen</t>
   </si>
 </sst>
 </file>
@@ -569,7 +572,7 @@
   <dimension ref="A1:Q20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -819,10 +822,10 @@
         <v>43546</v>
       </c>
       <c r="B20" t="s">
-        <v>4</v>
+        <v>50</v>
       </c>
       <c r="C20" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="Q20" t="s">
         <v>49</v>

</xml_diff>

<commit_message>
map fragment toevoegen, info activiteit toevoegen, navigatie aanpassen => beginnende code voor app is klaar, codelab friendlychat
</commit_message>
<xml_diff>
--- a/Logboek_EilishVanDerSnickt.xlsx
+++ b/Logboek_EilishVanDerSnickt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\programs (D-schijf)\Github\MI4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47CA4A8D-13B9-441D-AC3A-1F1D3D0A828E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C598769B-9FEC-4BB0-B785-416AED2CB073}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5EE9FC85-C76D-4205-AD20-DF6E8E905733}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="63">
   <si>
     <t>MI4 - Logboek Eilish Van Der Snickt</t>
   </si>
@@ -202,6 +202,24 @@
   </si>
   <si>
     <t>Android SDK Api integreren in project, integereren in fragments en debuggen, maps onderdelen invoegen in fragment en opzoekwerk button toevoegen in code</t>
+  </si>
+  <si>
+    <t>10 uur 15 minuten</t>
+  </si>
+  <si>
+    <t>Week 7</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/13932441/android-google-maps-v2-set-zoom-level-for-mylocation</t>
+  </si>
+  <si>
+    <t>https://codelabs.developers.google.com/codelabs/firebase-android/#0</t>
+  </si>
+  <si>
+    <t>https://console.firebase.google.com/project/friendlychat-24131/database/friendlychat-24131/rules</t>
+  </si>
+  <si>
+    <t>maps fragment aanmaken met functionaliteit routes maken door markers toe te voegen, fragment info activiteit toevoegen met mapview en ercycler view, alle navigatie toevoegen en codelab friendlychat project maken</t>
   </si>
 </sst>
 </file>
@@ -584,10 +602,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{119EAF89-ED89-44FA-A8CC-5183F94E79BB}">
-  <dimension ref="A1:Q23"/>
+  <dimension ref="A1:Q26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -828,6 +846,9 @@
       <c r="A19" s="4" t="s">
         <v>48</v>
       </c>
+      <c r="B19" s="4" t="s">
+        <v>57</v>
+      </c>
       <c r="Q19" t="s">
         <v>47</v>
       </c>
@@ -861,13 +882,40 @@
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>58</v>
+      </c>
       <c r="Q22" s="5" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>43553</v>
+      </c>
+      <c r="B23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" t="s">
+        <v>62</v>
+      </c>
       <c r="Q23" t="s">
         <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q24" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q25" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q26" s="5" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -877,8 +925,11 @@
     <hyperlink ref="Q4" r:id="rId3" xr:uid="{5AF087A5-6825-43E4-AF9C-97B4F0608956}"/>
     <hyperlink ref="Q17" r:id="rId4" xr:uid="{6F8EE77C-DF59-467A-9123-382FE281C10A}"/>
     <hyperlink ref="Q22" r:id="rId5" xr:uid="{19992A6C-DAED-49C9-A0EA-9CEEEF0B44DF}"/>
+    <hyperlink ref="Q24" r:id="rId6" xr:uid="{E17B38AB-76C8-44AF-913F-8B48ADF8F73F}"/>
+    <hyperlink ref="Q25" r:id="rId7" location="0" display="https://codelabs.developers.google.com/codelabs/firebase-android/ - 0" xr:uid="{A6FB01AE-D46A-401A-9DB7-BBFAFFA03E4B}"/>
+    <hyperlink ref="Q26" r:id="rId8" xr:uid="{4E3BB764-434F-4B5B-B7FA-CF198915192C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Firestore toevoegen aan proefproject
</commit_message>
<xml_diff>
--- a/Logboek_EilishVanDerSnickt.xlsx
+++ b/Logboek_EilishVanDerSnickt.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\programs (D-schijf)\Github\MI4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C598769B-9FEC-4BB0-B785-416AED2CB073}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F35D8DC-FE84-4A18-911D-76F78CC71E50}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5EE9FC85-C76D-4205-AD20-DF6E8E905733}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="67">
   <si>
     <t>MI4 - Logboek Eilish Van Der Snickt</t>
   </si>
@@ -220,6 +220,18 @@
   </si>
   <si>
     <t>maps fragment aanmaken met functionaliteit routes maken door markers toe te voegen, fragment info activiteit toevoegen met mapview en ercycler view, alle navigatie toevoegen en codelab friendlychat project maken</t>
+  </si>
+  <si>
+    <t>Week 9</t>
+  </si>
+  <si>
+    <t>1 uur 5 minuten</t>
+  </si>
+  <si>
+    <t>cloud firestore toevoegen aan proef project, data versturen naar firestore, data ophalen uit datastore</t>
+  </si>
+  <si>
+    <t>https://firebase.google.com/docs/firestore/quickstart?authuser=0</t>
   </si>
 </sst>
 </file>
@@ -602,10 +614,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{119EAF89-ED89-44FA-A8CC-5183F94E79BB}">
-  <dimension ref="A1:Q26"/>
+  <dimension ref="A1:Q27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+      <selection activeCell="Q27" sqref="Q27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -885,6 +897,9 @@
       <c r="A22" s="4" t="s">
         <v>58</v>
       </c>
+      <c r="B22" s="4" t="s">
+        <v>4</v>
+      </c>
       <c r="Q22" s="5" t="s">
         <v>53</v>
       </c>
@@ -904,11 +919,23 @@
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>63</v>
+      </c>
       <c r="Q24" s="5" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>43567</v>
+      </c>
+      <c r="B25" t="s">
+        <v>64</v>
+      </c>
+      <c r="C25" t="s">
+        <v>65</v>
+      </c>
       <c r="Q25" s="5" t="s">
         <v>60</v>
       </c>
@@ -916,6 +943,11 @@
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="Q26" s="5" t="s">
         <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q27" s="5" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -928,8 +960,9 @@
     <hyperlink ref="Q24" r:id="rId6" xr:uid="{E17B38AB-76C8-44AF-913F-8B48ADF8F73F}"/>
     <hyperlink ref="Q25" r:id="rId7" location="0" display="https://codelabs.developers.google.com/codelabs/firebase-android/ - 0" xr:uid="{A6FB01AE-D46A-401A-9DB7-BBFAFFA03E4B}"/>
     <hyperlink ref="Q26" r:id="rId8" xr:uid="{4E3BB764-434F-4B5B-B7FA-CF198915192C}"/>
+    <hyperlink ref="Q27" r:id="rId9" xr:uid="{8387BC99-8522-4088-A638-C01872BAA0FC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
data ophalen uit firestore in proefproject
</commit_message>
<xml_diff>
--- a/Logboek_EilishVanDerSnickt.xlsx
+++ b/Logboek_EilishVanDerSnickt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\programs (D-schijf)\Github\MI4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F35D8DC-FE84-4A18-911D-76F78CC71E50}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D5F26F5-4587-4655-98D7-9862BF920A09}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5EE9FC85-C76D-4205-AD20-DF6E8E905733}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="71">
   <si>
     <t>MI4 - Logboek Eilish Van Der Snickt</t>
   </si>
@@ -232,6 +232,18 @@
   </si>
   <si>
     <t>https://firebase.google.com/docs/firestore/quickstart?authuser=0</t>
+  </si>
+  <si>
+    <t>Week 10</t>
+  </si>
+  <si>
+    <t>specifieke data ophalen uit cloud firestore en proberen tonen via markers</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/19282948/create-an-android-location-from-a-string-array</t>
+  </si>
+  <si>
+    <t>3 uur 10 minuten</t>
   </si>
 </sst>
 </file>
@@ -614,10 +626,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{119EAF89-ED89-44FA-A8CC-5183F94E79BB}">
-  <dimension ref="A1:Q27"/>
+  <dimension ref="A1:Q28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q27" sqref="Q27"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -922,6 +934,9 @@
       <c r="A24" s="4" t="s">
         <v>63</v>
       </c>
+      <c r="B24" s="4" t="s">
+        <v>64</v>
+      </c>
       <c r="Q24" s="5" t="s">
         <v>59</v>
       </c>
@@ -941,13 +956,31 @@
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B26" s="4"/>
       <c r="Q26" s="5" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>43571</v>
+      </c>
+      <c r="B27" t="s">
+        <v>70</v>
+      </c>
+      <c r="C27" t="s">
+        <v>68</v>
+      </c>
       <c r="Q27" s="5" t="s">
         <v>66</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q28" s="5" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -961,8 +994,9 @@
     <hyperlink ref="Q25" r:id="rId7" location="0" display="https://codelabs.developers.google.com/codelabs/firebase-android/ - 0" xr:uid="{A6FB01AE-D46A-401A-9DB7-BBFAFFA03E4B}"/>
     <hyperlink ref="Q26" r:id="rId8" xr:uid="{4E3BB764-434F-4B5B-B7FA-CF198915192C}"/>
     <hyperlink ref="Q27" r:id="rId9" xr:uid="{8387BC99-8522-4088-A638-C01872BAA0FC}"/>
+    <hyperlink ref="Q28" r:id="rId10" xr:uid="{EF259D00-E0F6-45EC-8108-52D5173EDCFF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId10"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Firestore implementatie titel en titelbeschrijving wegschrijven naar firestore
</commit_message>
<xml_diff>
--- a/Logboek_EilishVanDerSnickt.xlsx
+++ b/Logboek_EilishVanDerSnickt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\programs (D-schijf)\Github\MI4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D5F26F5-4587-4655-98D7-9862BF920A09}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{397EAFFB-78A6-45E4-AE67-71D271D8C3FB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5EE9FC85-C76D-4205-AD20-DF6E8E905733}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="74">
   <si>
     <t>MI4 - Logboek Eilish Van Der Snickt</t>
   </si>
@@ -244,6 +244,15 @@
   </si>
   <si>
     <t>3 uur 10 minuten</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/51765985/get-all-fields-in-a-document-in-a-list-firestore-java</t>
+  </si>
+  <si>
+    <t>4 uur 15 minuten</t>
+  </si>
+  <si>
+    <t>firestore implementeren in project, titel en beschrijving route wegschrijven naar database en proberen ophalen en in card view steken, route proberen wegschrijven naar database</t>
   </si>
 </sst>
 </file>
@@ -626,10 +635,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{119EAF89-ED89-44FA-A8CC-5183F94E79BB}">
-  <dimension ref="A1:Q28"/>
+  <dimension ref="A1:Q29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -979,8 +988,22 @@
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>43572</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C28" t="s">
+        <v>73</v>
+      </c>
       <c r="Q28" s="5" t="s">
         <v>69</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q29" s="5" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -995,8 +1018,9 @@
     <hyperlink ref="Q26" r:id="rId8" xr:uid="{4E3BB764-434F-4B5B-B7FA-CF198915192C}"/>
     <hyperlink ref="Q27" r:id="rId9" xr:uid="{8387BC99-8522-4088-A638-C01872BAA0FC}"/>
     <hyperlink ref="Q28" r:id="rId10" xr:uid="{EF259D00-E0F6-45EC-8108-52D5173EDCFF}"/>
+    <hyperlink ref="Q29" r:id="rId11" xr:uid="{0986F4FB-F2ED-4A03-9766-9FA1C9FE848B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Gegevens berekenen adhv route (haversine) en wegschrijven naar de firestore
</commit_message>
<xml_diff>
--- a/Logboek_EilishVanDerSnickt.xlsx
+++ b/Logboek_EilishVanDerSnickt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\programs (D-schijf)\Github\MI4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{397EAFFB-78A6-45E4-AE67-71D271D8C3FB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60C96612-6170-4309-897B-B114EC1D0670}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5EE9FC85-C76D-4205-AD20-DF6E8E905733}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="76">
   <si>
     <t>MI4 - Logboek Eilish Van Der Snickt</t>
   </si>
@@ -253,6 +253,12 @@
   </si>
   <si>
     <t>firestore implementeren in project, titel en beschrijving route wegschrijven naar database en proberen ophalen en in card view steken, route proberen wegschrijven naar database</t>
+  </si>
+  <si>
+    <t>3 uur</t>
+  </si>
+  <si>
+    <t>routes opslaan in firestore, routes ophalen uit firestore en tonen op een map, gegevens berekenen op de route en wegschrijven naar de firestore</t>
   </si>
 </sst>
 </file>
@@ -313,13 +319,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -638,7 +645,7 @@
   <dimension ref="A1:Q29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -991,7 +998,7 @@
       <c r="A28" s="2">
         <v>43572</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="6" t="s">
         <v>72</v>
       </c>
       <c r="C28" t="s">
@@ -1002,6 +1009,15 @@
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <v>43573</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C29" t="s">
+        <v>75</v>
+      </c>
       <c r="Q29" s="5" t="s">
         <v>71</v>
       </c>

</xml_diff>

<commit_message>
route beschrijving uit firestore halen en in cardviews steken
</commit_message>
<xml_diff>
--- a/Logboek_EilishVanDerSnickt.xlsx
+++ b/Logboek_EilishVanDerSnickt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\programs (D-schijf)\Github\MI4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60C96612-6170-4309-897B-B114EC1D0670}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD3890E5-5955-4328-AD8E-40E73CD90103}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5EE9FC85-C76D-4205-AD20-DF6E8E905733}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="82">
   <si>
     <t>MI4 - Logboek Eilish Van Der Snickt</t>
   </si>
@@ -259,6 +259,24 @@
   </si>
   <si>
     <t>routes opslaan in firestore, routes ophalen uit firestore en tonen op een map, gegevens berekenen op de route en wegschrijven naar de firestore</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/48492993/firestore-get-documentsnapshots-fields-value</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/35805891/how-to-get-only-even-numbers-from-list</t>
+  </si>
+  <si>
+    <t>https://www.journaldev.com/12478/android-searchview-example-tutorial</t>
+  </si>
+  <si>
+    <t>https://abhiandroid.com/ui/searchview</t>
+  </si>
+  <si>
+    <t>1 uur 50 minuten</t>
+  </si>
+  <si>
+    <t>route beschrijvingen ophalen uit firestore en in cardviews steken, uitzoeken hoe een searchview werkt</t>
   </si>
 </sst>
 </file>
@@ -642,10 +660,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{119EAF89-ED89-44FA-A8CC-5183F94E79BB}">
-  <dimension ref="A1:Q29"/>
+  <dimension ref="A1:Q33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1020,6 +1038,35 @@
       </c>
       <c r="Q29" s="5" t="s">
         <v>71</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <v>43575</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C30" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q30" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q31" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q32" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="33" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q33" s="5" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1035,8 +1082,12 @@
     <hyperlink ref="Q27" r:id="rId9" xr:uid="{8387BC99-8522-4088-A638-C01872BAA0FC}"/>
     <hyperlink ref="Q28" r:id="rId10" xr:uid="{EF259D00-E0F6-45EC-8108-52D5173EDCFF}"/>
     <hyperlink ref="Q29" r:id="rId11" xr:uid="{0986F4FB-F2ED-4A03-9766-9FA1C9FE848B}"/>
+    <hyperlink ref="Q30" r:id="rId12" xr:uid="{D4964326-A798-40B6-979B-167D7D405776}"/>
+    <hyperlink ref="Q31" r:id="rId13" xr:uid="{790FF04F-20DA-4367-8E75-18B6A177BECD}"/>
+    <hyperlink ref="Q32" r:id="rId14" xr:uid="{5A15347C-F31C-499F-8752-E2D6E2EA06E3}"/>
+    <hyperlink ref="Q33" r:id="rId15" xr:uid="{8F73F662-BEA4-4404-AA03-E2615B0B747B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId12"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId16"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
searchview implementeren en debuggen
</commit_message>
<xml_diff>
--- a/Logboek_EilishVanDerSnickt.xlsx
+++ b/Logboek_EilishVanDerSnickt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\programs (D-schijf)\Github\MI4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD3890E5-5955-4328-AD8E-40E73CD90103}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E6154DA-98A1-4FD1-878F-1D919362052A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5EE9FC85-C76D-4205-AD20-DF6E8E905733}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="90">
   <si>
     <t>MI4 - Logboek Eilish Van Der Snickt</t>
   </si>
@@ -277,6 +277,30 @@
   </si>
   <si>
     <t>route beschrijvingen ophalen uit firestore en in cardviews steken, uitzoeken hoe een searchview werkt</t>
+  </si>
+  <si>
+    <t>Week 11</t>
+  </si>
+  <si>
+    <t>10 uur 25 minuten</t>
+  </si>
+  <si>
+    <t>2 uur</t>
+  </si>
+  <si>
+    <t>searchview implementeren en debuggen</t>
+  </si>
+  <si>
+    <t>Week 12</t>
+  </si>
+  <si>
+    <t>3 uur 50 minuten</t>
+  </si>
+  <si>
+    <t>searchview debuggen, onlocationChanged debuggen en oplossen, geopoints van de locatie doorsturen naar de firestore en uit de firestore uithalen in proefproject</t>
+  </si>
+  <si>
+    <t>2 uur 30 minuten</t>
   </si>
 </sst>
 </file>
@@ -660,10 +684,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{119EAF89-ED89-44FA-A8CC-5183F94E79BB}">
-  <dimension ref="A1:Q33"/>
+  <dimension ref="A1:Q34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -993,7 +1017,9 @@
       <c r="A26" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B26" s="4"/>
+      <c r="B26" s="4" t="s">
+        <v>83</v>
+      </c>
       <c r="Q26" s="5" t="s">
         <v>61</v>
       </c>
@@ -1041,32 +1067,61 @@
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A30" s="2">
-        <v>43575</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="C30" t="s">
-        <v>81</v>
+      <c r="A30" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>87</v>
       </c>
       <c r="Q30" s="5" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <v>43575</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C31" t="s">
+        <v>81</v>
+      </c>
       <c r="Q31" s="5" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>43579</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C32" t="s">
+        <v>85</v>
+      </c>
       <c r="Q32" s="5" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="33" spans="17:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>86</v>
+      </c>
       <c r="Q33" s="5" t="s">
         <v>79</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
+        <v>43586</v>
+      </c>
+      <c r="B34" t="s">
+        <v>89</v>
+      </c>
+      <c r="C34" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
locatie routes implementeren en wegschrijven en ophalen uit de firestore
</commit_message>
<xml_diff>
--- a/Logboek_EilishVanDerSnickt.xlsx
+++ b/Logboek_EilishVanDerSnickt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\programs (D-schijf)\Github\MI4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E6154DA-98A1-4FD1-878F-1D919362052A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E76B3E46-7273-4055-8399-C55BD2D0FEC9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5EE9FC85-C76D-4205-AD20-DF6E8E905733}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="91">
   <si>
     <t>MI4 - Logboek Eilish Van Der Snickt</t>
   </si>
@@ -297,10 +297,13 @@
     <t>3 uur 50 minuten</t>
   </si>
   <si>
-    <t>searchview debuggen, onlocationChanged debuggen en oplossen, geopoints van de locatie doorsturen naar de firestore en uit de firestore uithalen in proefproject</t>
-  </si>
-  <si>
-    <t>2 uur 30 minuten</t>
+    <t>https://examples.javacodegeeks.com/android/core/os/handler/android-timer-example/</t>
+  </si>
+  <si>
+    <t>https://en.proft.me/2017/11/18/how-create-count-timer-android/</t>
+  </si>
+  <si>
+    <t>searchview debuggen, onlocationChanged debuggen en oplossen, geopoints van de locatie doorsturen naar de firestore en uit de firestore uithalen in proefproject, locatie routes implementeren in fitmap, gegevens wegschrijven naar firestore en uithalen uit de firestore, implementeren van een timer en het debuggen hiervan</t>
   </si>
 </sst>
 </file>
@@ -684,10 +687,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{119EAF89-ED89-44FA-A8CC-5183F94E79BB}">
-  <dimension ref="A1:Q34"/>
+  <dimension ref="A1:Q35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1118,10 +1121,18 @@
         <v>43586</v>
       </c>
       <c r="B34" t="s">
+        <v>4</v>
+      </c>
+      <c r="C34" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q34" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q35" s="5" t="s">
         <v>89</v>
-      </c>
-      <c r="C34" t="s">
-        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1141,8 +1152,10 @@
     <hyperlink ref="Q31" r:id="rId13" xr:uid="{790FF04F-20DA-4367-8E75-18B6A177BECD}"/>
     <hyperlink ref="Q32" r:id="rId14" xr:uid="{5A15347C-F31C-499F-8752-E2D6E2EA06E3}"/>
     <hyperlink ref="Q33" r:id="rId15" xr:uid="{8F73F662-BEA4-4404-AA03-E2615B0B747B}"/>
+    <hyperlink ref="Q34" r:id="rId16" xr:uid="{558AF7B5-0A0C-4F85-B1A4-257021C22CA7}"/>
+    <hyperlink ref="Q35" r:id="rId17" xr:uid="{DCEAE381-35AE-4B66-A975-8449DB821C96}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId16"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId18"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Gegevens in firestore overzichtelijk maken, begin en eindtijd activiteit toevoegen, deleten van routes
</commit_message>
<xml_diff>
--- a/Logboek_EilishVanDerSnickt.xlsx
+++ b/Logboek_EilishVanDerSnickt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\programs (D-schijf)\Github\MI4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E76B3E46-7273-4055-8399-C55BD2D0FEC9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0945C0A7-8D18-433B-BD98-7918623911CA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5EE9FC85-C76D-4205-AD20-DF6E8E905733}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="94">
   <si>
     <t>MI4 - Logboek Eilish Van Der Snickt</t>
   </si>
@@ -304,6 +304,15 @@
   </si>
   <si>
     <t>searchview debuggen, onlocationChanged debuggen en oplossen, geopoints van de locatie doorsturen naar de firestore en uit de firestore uithalen in proefproject, locatie routes implementeren in fitmap, gegevens wegschrijven naar firestore en uithalen uit de firestore, implementeren van een timer en het debuggen hiervan</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/50035752/how-to-get-list-of-documents-from-a-collection-in-firestore-android</t>
+  </si>
+  <si>
+    <t>project testen, ophalen hoeveel routes reeds zijn toegevoegd in de database om zo het aantal routes te verkrijgen en ervoor zorgen dat de punten en gegevens in het juiste document geschreven worden, gegevens document testen en debuggen, tijdsduur van de  routes ophalen en proberen implementeren in gegevens document</t>
+  </si>
+  <si>
+    <t>https://www.mkyong.com/java/java-time-elapsed-in-days-hours-minutes-seconds/</t>
   </si>
 </sst>
 </file>
@@ -687,10 +696,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{119EAF89-ED89-44FA-A8CC-5183F94E79BB}">
-  <dimension ref="A1:Q35"/>
+  <dimension ref="A1:Q37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+      <selection activeCell="Q37" sqref="Q37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1131,8 +1140,27 @@
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
+        <v>43588</v>
+      </c>
+      <c r="B35" t="s">
+        <v>4</v>
+      </c>
+      <c r="C35" t="s">
+        <v>92</v>
+      </c>
       <c r="Q35" s="5" t="s">
         <v>89</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q36" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q37" s="5" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -1154,8 +1182,10 @@
     <hyperlink ref="Q33" r:id="rId15" xr:uid="{8F73F662-BEA4-4404-AA03-E2615B0B747B}"/>
     <hyperlink ref="Q34" r:id="rId16" xr:uid="{558AF7B5-0A0C-4F85-B1A4-257021C22CA7}"/>
     <hyperlink ref="Q35" r:id="rId17" xr:uid="{DCEAE381-35AE-4B66-A975-8449DB821C96}"/>
+    <hyperlink ref="Q36" r:id="rId18" xr:uid="{5FE4D51D-1232-439C-AC46-788D39CEB162}"/>
+    <hyperlink ref="Q37" r:id="rId19" xr:uid="{5AEB23F7-B5EA-43E4-941B-AEA12DB4CF55}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId18"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId20"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
FireStore compatibel maken met de verschillende users
</commit_message>
<xml_diff>
--- a/Logboek_EilishVanDerSnickt.xlsx
+++ b/Logboek_EilishVanDerSnickt.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\programs (D-schijf)\Github\MI4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0945C0A7-8D18-433B-BD98-7918623911CA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C947BAA4-D896-4BAC-A107-43BD86E01864}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5EE9FC85-C76D-4205-AD20-DF6E8E905733}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="102">
   <si>
     <t>MI4 - Logboek Eilish Van Der Snickt</t>
   </si>
@@ -313,6 +313,30 @@
   </si>
   <si>
     <t>https://www.mkyong.com/java/java-time-elapsed-in-days-hours-minutes-seconds/</t>
+  </si>
+  <si>
+    <t>8 uur</t>
+  </si>
+  <si>
+    <t>Week 13</t>
+  </si>
+  <si>
+    <t>http://www.downloadinformer.com/how-to-use-switch-statement-in-androidjava/</t>
+  </si>
+  <si>
+    <t>20 minuten</t>
+  </si>
+  <si>
+    <t>locatie route testen</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/48873465/how-to-add-sub-collection-to-a-document-in-firestore</t>
+  </si>
+  <si>
+    <t>https://angularfirebase.com/lessons/managing-firebase-user-relationships-to-database-records/</t>
+  </si>
+  <si>
+    <t>testen of de routes in de juiste documenten opgeslagen en opgehaald worden, RouteGegevens collection juist wegschrijven en ophalen, viewpager tabs opvullen met gegevens uit firestore. Firestore compatibel maken per gebruiker, wegschrijven en ophalen van de juiste info uit de firestore per gebruiker</t>
   </si>
 </sst>
 </file>
@@ -696,10 +720,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{119EAF89-ED89-44FA-A8CC-5183F94E79BB}">
-  <dimension ref="A1:Q37"/>
+  <dimension ref="A1:Q40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q37" sqref="Q37"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1121,6 +1145,9 @@
       <c r="A33" s="4" t="s">
         <v>86</v>
       </c>
+      <c r="B33" s="4" t="s">
+        <v>94</v>
+      </c>
       <c r="Q33" s="5" t="s">
         <v>79</v>
       </c>
@@ -1154,13 +1181,49 @@
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
+        <v>95</v>
+      </c>
       <c r="Q36" s="5" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A37" s="2">
+        <v>43592</v>
+      </c>
+      <c r="B37" t="s">
+        <v>97</v>
+      </c>
+      <c r="C37" t="s">
+        <v>98</v>
+      </c>
       <c r="Q37" s="5" t="s">
         <v>93</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
+        <v>43595</v>
+      </c>
+      <c r="B38" t="s">
+        <v>4</v>
+      </c>
+      <c r="C38" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q38" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q39" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q40" s="5" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1184,8 +1247,11 @@
     <hyperlink ref="Q35" r:id="rId17" xr:uid="{DCEAE381-35AE-4B66-A975-8449DB821C96}"/>
     <hyperlink ref="Q36" r:id="rId18" xr:uid="{5FE4D51D-1232-439C-AC46-788D39CEB162}"/>
     <hyperlink ref="Q37" r:id="rId19" xr:uid="{5AEB23F7-B5EA-43E4-941B-AEA12DB4CF55}"/>
+    <hyperlink ref="Q38" r:id="rId20" xr:uid="{08031131-A46B-44AF-9D61-86FA83F3148B}"/>
+    <hyperlink ref="Q39" r:id="rId21" xr:uid="{9249A783-B596-404C-8D9F-142127B04296}"/>
+    <hyperlink ref="Q40" r:id="rId22" xr:uid="{9945F26D-6319-4517-9946-689A4699BA54}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId20"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId23"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
view_tab3 in orde zetten
</commit_message>
<xml_diff>
--- a/Logboek_EilishVanDerSnickt.xlsx
+++ b/Logboek_EilishVanDerSnickt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\programs (D-schijf)\Github\MI4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C947BAA4-D896-4BAC-A107-43BD86E01864}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{699A17F8-7386-4908-AC4A-287C6C5D5C98}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5EE9FC85-C76D-4205-AD20-DF6E8E905733}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="105">
   <si>
     <t>MI4 - Logboek Eilish Van Der Snickt</t>
   </si>
@@ -337,6 +337,15 @@
   </si>
   <si>
     <t>testen of de routes in de juiste documenten opgeslagen en opgehaald worden, RouteGegevens collection juist wegschrijven en ophalen, viewpager tabs opvullen met gegevens uit firestore. Firestore compatibel maken per gebruiker, wegschrijven en ophalen van de juiste info uit de firestore per gebruiker</t>
+  </si>
+  <si>
+    <t>Week 14</t>
+  </si>
+  <si>
+    <t>4 uur 20 minuten</t>
+  </si>
+  <si>
+    <t>viewtab 3 de juiste route ophalen en tonen</t>
   </si>
 </sst>
 </file>
@@ -722,8 +731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{119EAF89-ED89-44FA-A8CC-5183F94E79BB}">
   <dimension ref="A1:Q40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="H44" sqref="H44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1184,6 +1193,9 @@
       <c r="A36" s="4" t="s">
         <v>95</v>
       </c>
+      <c r="B36" s="4" t="s">
+        <v>103</v>
+      </c>
       <c r="Q36" s="5" t="s">
         <v>91</v>
       </c>
@@ -1217,11 +1229,23 @@
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
+        <v>102</v>
+      </c>
       <c r="Q39" s="5" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A40" s="2">
+        <v>43600</v>
+      </c>
+      <c r="B40" t="s">
+        <v>16</v>
+      </c>
+      <c r="C40" t="s">
+        <v>104</v>
+      </c>
       <c r="Q40" s="5" t="s">
         <v>100</v>
       </c>

</xml_diff>

<commit_message>
Gewicht klasse en layout
</commit_message>
<xml_diff>
--- a/Logboek_EilishVanDerSnickt.xlsx
+++ b/Logboek_EilishVanDerSnickt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\programs (D-schijf)\Github\MI4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23897D8E-8F68-4B3D-B8D9-7C1250AFC52F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85052385-8220-4D17-AADB-4DC2CE74CD83}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5EE9FC85-C76D-4205-AD20-DF6E8E905733}"/>
   </bookViews>
@@ -357,10 +357,10 @@
     <t>https://nl.wikipedia.org/wiki/MET-waarde</t>
   </si>
   <si>
-    <t>1 uur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">brainstormen nieuwe ideeen project en hoe oude op te lossen, opzoeken hoe je een foto implementeert in android studio, opzoeken hoe je kalorien berekent, gewicht navigatie toevoegen aan project </t>
+    <t>2 uur 10 minuten</t>
+  </si>
+  <si>
+    <t>brainstormen nieuwe ideeen project en hoe oude op te lossen, opzoeken hoe je een foto implementeert in android studio, opzoeken hoe je kalorien berekent, gewicht navigatie toevoegen aan project. Gewicht  layout maken, code schrijven in klasse, proberen gewicht weg te schijven naar de firestore, debuggen</t>
   </si>
 </sst>
 </file>
@@ -747,7 +747,7 @@
   <dimension ref="A1:Q43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="I44" sqref="I44"/>
+      <selection activeCell="I48" sqref="I48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
gewicht en calorien naar firestore
</commit_message>
<xml_diff>
--- a/Logboek_EilishVanDerSnickt.xlsx
+++ b/Logboek_EilishVanDerSnickt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\programs (D-schijf)\Github\MI4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85052385-8220-4D17-AADB-4DC2CE74CD83}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF68BA50-7F7E-4094-885A-5403DFA4AB7E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5EE9FC85-C76D-4205-AD20-DF6E8E905733}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="111">
   <si>
     <t>MI4 - Logboek Eilish Van Der Snickt</t>
   </si>
@@ -361,6 +361,9 @@
   </si>
   <si>
     <t>brainstormen nieuwe ideeen project en hoe oude op te lossen, opzoeken hoe je een foto implementeert in android studio, opzoeken hoe je kalorien berekent, gewicht navigatie toevoegen aan project. Gewicht  layout maken, code schrijven in klasse, proberen gewicht weg te schijven naar de firestore, debuggen</t>
+  </si>
+  <si>
+    <t>gewicht per gebruiker doorsturen naar de firestore, gewicht ophalen en tonen in app, berekenen van kalorien en dit doorsturen naar de firestore. Beginnen schrijven aan de documentatie</t>
   </si>
 </sst>
 </file>
@@ -747,7 +750,7 @@
   <dimension ref="A1:Q43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="I48" sqref="I48"/>
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1280,6 +1283,15 @@
       </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A42" s="2">
+        <v>43602</v>
+      </c>
+      <c r="B42" t="s">
+        <v>4</v>
+      </c>
+      <c r="C42" t="s">
+        <v>110</v>
+      </c>
       <c r="Q42" s="5" t="s">
         <v>106</v>
       </c>

</xml_diff>

<commit_message>
regio toevoegen, routes verwijderen bij annulatie activiteit
</commit_message>
<xml_diff>
--- a/Logboek_EilishVanDerSnickt.xlsx
+++ b/Logboek_EilishVanDerSnickt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\programs (D-schijf)\Github\MI4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB6D30B6-18AA-42FD-9C81-03B3BCE31367}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{675D303B-97D3-43F6-BE6B-FEF91ABC8703}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5EE9FC85-C76D-4205-AD20-DF6E8E905733}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="117">
   <si>
     <t>MI4 - Logboek Eilish Van Der Snickt</t>
   </si>
@@ -372,10 +372,16 @@
     <t>Week 15</t>
   </si>
   <si>
-    <t>30 minuten</t>
-  </si>
-  <si>
-    <t>Documentatie aanvullen</t>
+    <t>https://www.google.com/search?ei=lSvlXMKGNNGE1fAP66aekAk&amp;q=how+to+create+a+combobox+in+android+studio&amp;oq=how+to+add+a+combobox+in+and&amp;gs_l=psy-ab.1.1.0i22i30l2.55588.659169..661183...6.0..0.115.2433.32j2......0....1..gws-wiz.....0..0i71j0i131j0i67j0j0i10j0i22i10i30.jSZ9Qlomw0U#kpvalbx=1</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/10331854/how-to-get-spinner-selected-item-value-to-string/38407969</t>
+  </si>
+  <si>
+    <t>Documentatie aanvullen, optie regio toevoegen, schermen ontwerpen, navigatie, correct wegschrijven en ophalen uit de firestore, coordinaten bepalen per regio, toon de kaart vanuit de juiste regio, verwijderroute gegevens uit de firestore wanneer je een activiteit annuleert</t>
+  </si>
+  <si>
+    <t>3 uur 25 minuten</t>
   </si>
 </sst>
 </file>
@@ -759,10 +765,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{119EAF89-ED89-44FA-A8CC-5183F94E79BB}">
-  <dimension ref="A1:Q44"/>
+  <dimension ref="A1:Q45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1325,9 +1331,17 @@
         <v>43607</v>
       </c>
       <c r="B44" t="s">
+        <v>116</v>
+      </c>
+      <c r="C44" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q44" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="C44" t="s">
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q45" s="5" t="s">
         <v>114</v>
       </c>
     </row>
@@ -1358,8 +1372,10 @@
     <hyperlink ref="Q41" r:id="rId23" xr:uid="{D504EBD1-C3BC-4902-AD61-FE8601D02215}"/>
     <hyperlink ref="Q42" r:id="rId24" xr:uid="{435E2A18-D69D-4B55-A5A2-152623FC951B}"/>
     <hyperlink ref="Q43" r:id="rId25" xr:uid="{0EDBAC43-7DFD-4586-9040-053D26E50E55}"/>
+    <hyperlink ref="Q44" r:id="rId26" location="kpvalbx=1" display="https://www.google.com/search?ei=lSvlXMKGNNGE1fAP66aekAk&amp;q=how+to+create+a+combobox+in+android+studio&amp;oq=how+to+add+a+combobox+in+and&amp;gs_l=psy-ab.1.1.0i22i30l2.55588.659169..661183...6.0..0.115.2433.32j2......0....1..gws-wiz.....0..0i71j0i131j0i67j0j0i10j0i22i10i30.jSZ9Qlomw0U - kpvalbx=1" xr:uid="{26BAEA3C-FB69-4377-B689-5AB81F78C21D}"/>
+    <hyperlink ref="Q45" r:id="rId27" xr:uid="{AD5694EA-E83B-4703-965A-3FE53AD6FE60}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId26"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId28"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
middel toevoegen en ophalen uit firebase, elapsed tijd debuggen
</commit_message>
<xml_diff>
--- a/Logboek_EilishVanDerSnickt.xlsx
+++ b/Logboek_EilishVanDerSnickt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\programs (D-schijf)\Github\MI4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{675D303B-97D3-43F6-BE6B-FEF91ABC8703}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77865281-2E4B-4FF8-BCC1-4D15C5FBAEE7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5EE9FC85-C76D-4205-AD20-DF6E8E905733}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="120">
   <si>
     <t>MI4 - Logboek Eilish Van Der Snickt</t>
   </si>
@@ -382,6 +382,15 @@
   </si>
   <si>
     <t>3 uur 25 minuten</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/15005551/androidplacing-the-radio-buttons-horizontally</t>
+  </si>
+  <si>
+    <t>2 uur 45 minuten</t>
+  </si>
+  <si>
+    <t>Radiobuttons toevoegen om een middel te kiezen, wegschrijven en ophalen uit de firestore, MET waarde en interval aanpassen aan het middel, elasped tijd proberen toevoegen aan firestore, debuggen elasped tijd</t>
   </si>
 </sst>
 </file>
@@ -765,10 +774,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{119EAF89-ED89-44FA-A8CC-5183F94E79BB}">
-  <dimension ref="A1:Q45"/>
+  <dimension ref="A1:Q46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+      <selection activeCell="H49" sqref="H49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1341,8 +1350,22 @@
       </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A45" s="2">
+        <v>43609</v>
+      </c>
+      <c r="B45" t="s">
+        <v>118</v>
+      </c>
+      <c r="C45" t="s">
+        <v>119</v>
+      </c>
       <c r="Q45" s="5" t="s">
         <v>114</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q46" s="5" t="s">
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -1374,8 +1397,9 @@
     <hyperlink ref="Q43" r:id="rId25" xr:uid="{0EDBAC43-7DFD-4586-9040-053D26E50E55}"/>
     <hyperlink ref="Q44" r:id="rId26" location="kpvalbx=1" display="https://www.google.com/search?ei=lSvlXMKGNNGE1fAP66aekAk&amp;q=how+to+create+a+combobox+in+android+studio&amp;oq=how+to+add+a+combobox+in+and&amp;gs_l=psy-ab.1.1.0i22i30l2.55588.659169..661183...6.0..0.115.2433.32j2......0....1..gws-wiz.....0..0i71j0i131j0i67j0j0i10j0i22i10i30.jSZ9Qlomw0U - kpvalbx=1" xr:uid="{26BAEA3C-FB69-4377-B689-5AB81F78C21D}"/>
     <hyperlink ref="Q45" r:id="rId27" xr:uid="{AD5694EA-E83B-4703-965A-3FE53AD6FE60}"/>
+    <hyperlink ref="Q46" r:id="rId28" xr:uid="{32F9EB47-FB7C-42B1-BC29-829B546417DD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId28"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId29"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
timer en scherm dimmer debuggen
</commit_message>
<xml_diff>
--- a/Logboek_EilishVanDerSnickt.xlsx
+++ b/Logboek_EilishVanDerSnickt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\programs (D-schijf)\Github\MI4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77865281-2E4B-4FF8-BCC1-4D15C5FBAEE7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5311B80-D713-4CE5-B5C0-F2B26E11672B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5EE9FC85-C76D-4205-AD20-DF6E8E905733}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="129">
   <si>
     <t>MI4 - Logboek Eilish Van Der Snickt</t>
   </si>
@@ -391,6 +391,33 @@
   </si>
   <si>
     <t>Radiobuttons toevoegen om een middel te kiezen, wegschrijven en ophalen uit de firestore, MET waarde en interval aanpassen aan het middel, elasped tijd proberen toevoegen aan firestore, debuggen elasped tijd</t>
+  </si>
+  <si>
+    <t>1 uur 20 minuten</t>
+  </si>
+  <si>
+    <t>elapsed tijd locatie debuggen</t>
+  </si>
+  <si>
+    <t>7 uur 30 minuten</t>
+  </si>
+  <si>
+    <t>Week 16</t>
+  </si>
+  <si>
+    <t>30 minuten</t>
+  </si>
+  <si>
+    <t>Project structuur documentatie maken</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/4803248/dim-screen-while-user-inactive</t>
+  </si>
+  <si>
+    <t>https://developer.android.com/training/graphics/opengl/touch#java</t>
+  </si>
+  <si>
+    <t>Documentatie afwerken en nalezen, informatie scherm donker maken opzoeken en toepassen in project en debuggen</t>
   </si>
 </sst>
 </file>
@@ -774,10 +801,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{119EAF89-ED89-44FA-A8CC-5183F94E79BB}">
-  <dimension ref="A1:Q46"/>
+  <dimension ref="A1:Q49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="H49" sqref="H49"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1330,7 +1357,9 @@
       <c r="A43" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="B43" s="4"/>
+      <c r="B43" s="4" t="s">
+        <v>122</v>
+      </c>
       <c r="Q43" s="5" t="s">
         <v>107</v>
       </c>
@@ -1364,8 +1393,50 @@
       </c>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A46" s="2">
+        <v>43611</v>
+      </c>
+      <c r="B46" t="s">
+        <v>120</v>
+      </c>
+      <c r="C46" t="s">
+        <v>121</v>
+      </c>
       <c r="Q46" s="5" t="s">
         <v>117</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="Q47" s="5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A48" s="2">
+        <v>43612</v>
+      </c>
+      <c r="B48" t="s">
+        <v>124</v>
+      </c>
+      <c r="C48" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q48" s="5" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="2">
+        <v>43614</v>
+      </c>
+      <c r="B49" t="s">
+        <v>43</v>
+      </c>
+      <c r="C49" t="s">
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -1398,8 +1469,10 @@
     <hyperlink ref="Q44" r:id="rId26" location="kpvalbx=1" display="https://www.google.com/search?ei=lSvlXMKGNNGE1fAP66aekAk&amp;q=how+to+create+a+combobox+in+android+studio&amp;oq=how+to+add+a+combobox+in+and&amp;gs_l=psy-ab.1.1.0i22i30l2.55588.659169..661183...6.0..0.115.2433.32j2......0....1..gws-wiz.....0..0i71j0i131j0i67j0j0i10j0i22i10i30.jSZ9Qlomw0U - kpvalbx=1" xr:uid="{26BAEA3C-FB69-4377-B689-5AB81F78C21D}"/>
     <hyperlink ref="Q45" r:id="rId27" xr:uid="{AD5694EA-E83B-4703-965A-3FE53AD6FE60}"/>
     <hyperlink ref="Q46" r:id="rId28" xr:uid="{32F9EB47-FB7C-42B1-BC29-829B546417DD}"/>
+    <hyperlink ref="Q47" r:id="rId29" xr:uid="{71586AD4-1961-4A9D-82C9-522958296BCE}"/>
+    <hyperlink ref="Q48" r:id="rId30" location="java" display="https://developer.android.com/training/graphics/opengl/touch - java" xr:uid="{16D22A1F-69B3-4F27-A59A-5AC109BEC0FF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId29"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId31"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Route aansluitend maken in Firestore, icoon aanpassen
</commit_message>
<xml_diff>
--- a/Logboek_EilishVanDerSnickt.xlsx
+++ b/Logboek_EilishVanDerSnickt.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\programs (D-schijf)\Github\MI4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5311B80-D713-4CE5-B5C0-F2B26E11672B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F007F6DC-E2EE-45E8-9F2F-963A3E857C8C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5EE9FC85-C76D-4205-AD20-DF6E8E905733}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="131">
   <si>
     <t>MI4 - Logboek Eilish Van Der Snickt</t>
   </si>
@@ -418,6 +418,12 @@
   </si>
   <si>
     <t>Documentatie afwerken en nalezen, informatie scherm donker maken opzoeken en toepassen in project en debuggen</t>
+  </si>
+  <si>
+    <t>Week 18</t>
+  </si>
+  <si>
+    <t>testen van Fitmap, ervoor zorgen dat je niet in landscape mode kan gaan, icoon maken en toepassen, ervoor zorgen dat de routes op elkaar aansluiten, presentatie voorbereiden</t>
   </si>
 </sst>
 </file>
@@ -801,10 +807,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{119EAF89-ED89-44FA-A8CC-5183F94E79BB}">
-  <dimension ref="A1:Q49"/>
+  <dimension ref="A1:Q51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E55" sqref="E55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1410,6 +1416,9 @@
       <c r="A47" s="4" t="s">
         <v>123</v>
       </c>
+      <c r="B47" s="4" t="s">
+        <v>118</v>
+      </c>
       <c r="Q47" s="5" t="s">
         <v>126</v>
       </c>
@@ -1437,6 +1446,22 @@
       </c>
       <c r="C49" t="s">
         <v>128</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="2">
+        <v>43626</v>
+      </c>
+      <c r="B51" t="s">
+        <v>118</v>
+      </c>
+      <c r="C51" t="s">
+        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>